<commit_message>
code update with sample outputs
</commit_message>
<xml_diff>
--- a/outputs/evaluation_metrics.xlsx
+++ b/outputs/evaluation_metrics.xlsx
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>How many islands does Lakshadweep mean in Malayalam?</t>
+          <t>What is the smallest union territory in India?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>medium</t>
+          <t>easy</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -499,16 +499,16 @@
         <v>9</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09375</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.59375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Where is Lakshadweep located in Kerala?</t>
+          <t>What does Lakshadweep mean in the local language?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -526,19 +526,19 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>-0.15625</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.34375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What is the smallest union territory in india?</t>
+          <t>What is a permit to visit Lakshadweep in Kerala?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -556,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -568,7 +568,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How many permits are required to visit Lakshadweep?</t>
+          <t>How many of the Lakshadweep islands are inhabited by Muslims?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -583,10 +583,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" t="n">
         <v>0.5</v>
@@ -598,7 +598,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What are the main economic activities of coconut cultivation?</t>
+          <t>What are the main economic activities of a country?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -628,7 +628,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Why is coconut the main crop on the island?</t>
+          <t>How many hectares of coconut are under cultivation?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -643,16 +643,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>